<commit_message>
Final tweaks before test
</commit_message>
<xml_diff>
--- a/Docs/Buzzer System BOM.xlsx
+++ b/Docs/Buzzer System BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colytongrammarschool-my.sharepoint.com/personal/18rmitcham_colytongrammar_com/Documents/A-Levels/Other/Buzzer System/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colytongrammarschool-my.sharepoint.com/personal/18rmitcham_colytongrammar_com/Documents/A-Levels/Other/Buzzer System/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{540CE541-DD81-4544-BFC3-1DC1AAF319E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28DBFC2C-3476-4B03-9ACE-A9CAE6E003B3}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{540CE541-DD81-4544-BFC3-1DC1AAF319E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91E07B3A-935F-4BD3-B0FC-7DD17A1B2AD6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{84CFF804-1E87-47D5-814C-F7C178BC3692}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84CFF804-1E87-47D5-814C-F7C178BC3692}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,10 +88,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,20 +193,20 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -228,10 +228,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +273,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +379,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,11 +531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7185EFC-2C7E-4C20-A40D-BB382D04D37F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
@@ -542,7 +546,7 @@
     <col min="8" max="8" width="100.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -568,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -586,7 +590,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="5">
-        <f t="shared" ref="F2:F6" si="1">B2*E2</f>
+        <f t="shared" ref="F2:F5" si="1">B2*E2</f>
         <v>24</v>
       </c>
       <c r="G2" t="s">
@@ -597,7 +601,7 @@
         <v>https://thepihut.com/products/2-x-aaa-open-battery-holder-with-jst-ph-connector</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -626,7 +630,7 @@
         <v>https://thepihut.com/products/neopixel-diffused-8mm-through-hole-led-5-pack?variant=27739588177</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -654,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -679,11 +683,11 @@
         <v>12</v>
       </c>
       <c r="H5" s="3" t="str">
-        <f>HYPERLINK("https://shorturl.at/ALPX4")</f>
-        <v>https://shorturl.at/ALPX4</v>
+        <f>HYPERLINK("https:/shorturl.at/ALPX4")</f>
+        <v>https:/shorturl.at/ALPX4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="E6" s="4"/>
@@ -693,10 +697,10 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a far throw client
</commit_message>
<xml_diff>
--- a/Docs/Buzzer System BOM.xlsx
+++ b/Docs/Buzzer System BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colytongrammarschool-my.sharepoint.com/personal/18rmitcham_colytongrammar_com/Documents/A-Levels/Other/Buzzer System/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{540CE541-DD81-4544-BFC3-1DC1AAF319E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91E07B3A-935F-4BD3-B0FC-7DD17A1B2AD6}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{540CE541-DD81-4544-BFC3-1DC1AAF319E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1800F090-03AD-4BA7-8EC5-059B5BBF15A2}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84CFF804-1E87-47D5-814C-F7C178BC3692}"/>
   </bookViews>
@@ -226,10 +226,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7185EFC-2C7E-4C20-A40D-BB382D04D37F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +611,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(D3/C3, 0)</f>
         <v>4</v>
       </c>
       <c r="F3" s="5">

</xml_diff>